<commit_message>
Added Links for Talents
</commit_message>
<xml_diff>
--- a/Docs/Kickoff Talent Skills Spreadsheet.xlsx
+++ b/Docs/Kickoff Talent Skills Spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28717"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\6th Semester\SPM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Semester 6\SPM\Project\OrderEase\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768C52DB-C120-486D-B9B9-7D8961E02559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4CDD36-831F-43CE-A95C-479230FA4252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
   <si>
     <t>Skill Needed</t>
   </si>
@@ -86,9 +86,6 @@
     <t>Abdul Rehman-57</t>
   </si>
   <si>
-    <t>React.js, Next.js, JavaScript, HTML, CSS</t>
-  </si>
-  <si>
     <t>Mudasir Ahmed</t>
   </si>
   <si>
@@ -119,9 +116,6 @@
     <t>Testing/QA</t>
   </si>
   <si>
-    <t>Selenium</t>
-  </si>
-  <si>
     <t>Documentation</t>
   </si>
   <si>
@@ -132,9 +126,6 @@
   </si>
   <si>
     <t>Deployment</t>
-  </si>
-  <si>
-    <t>Heroku, Netlify, Vercel</t>
   </si>
   <si>
     <t>SEO</t>
@@ -168,6 +159,12 @@
   </si>
   <si>
     <t>https://drive.google.com/drive/folders/1G4oPspZPaFH-ThmHbAVUpu9BfIiQy3Ee?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://movie-browser-coral.vercel.app/</t>
+  </si>
+  <si>
+    <t>https://github.com/AbdulRehmani2/twitter</t>
   </si>
 </sst>
 </file>
@@ -491,6 +488,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -517,13 +521,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -936,25 +933,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY417"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.08203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.58203125" customWidth="1"/>
+    <col min="4" max="4" width="4.625" customWidth="1"/>
     <col min="5" max="5" width="20.25" customWidth="1"/>
     <col min="6" max="6" width="28.25" customWidth="1"/>
-    <col min="7" max="7" width="41.4140625" customWidth="1"/>
-    <col min="8" max="8" width="25.58203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="41.375" customWidth="1"/>
+    <col min="8" max="8" width="25.625" style="1" customWidth="1"/>
     <col min="9" max="9" width="14.25" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.75" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:51" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -969,24 +966,24 @@
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
     </row>
-    <row r="2" spans="1:51" s="1" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="1.3">
+    <row r="2" spans="1:51" s="1" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:51" s="1" customFormat="1" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:51" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6"/>
       <c r="B3" s="10" t="s">
         <v>9</v>
@@ -996,18 +993,18 @@
       <c r="E3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="32" t="s">
-        <v>43</v>
+      <c r="F3" s="35" t="s">
+        <v>40</v>
       </c>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
     </row>
-    <row r="4" spans="1:51" s="1" customFormat="1" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:51" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -1015,18 +1012,18 @@
       <c r="E4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="34" t="s">
-        <v>41</v>
+      <c r="F4" s="37" t="s">
+        <v>38</v>
       </c>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
     </row>
-    <row r="5" spans="1:51" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="11"/>
       <c r="C5" s="12"/>
@@ -1079,7 +1076,7 @@
       <c r="AX5" s="1"/>
       <c r="AY5" s="1"/>
     </row>
-    <row r="6" spans="1:51" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:51" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="25" t="s">
         <v>3</v>
@@ -1144,7 +1141,7 @@
       <c r="AX6" s="1"/>
       <c r="AY6" s="1"/>
     </row>
-    <row r="7" spans="1:51" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="2">
         <v>1</v>
@@ -1159,8 +1156,8 @@
       <c r="F7" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="17" t="s">
-        <v>19</v>
+      <c r="G7" s="27" t="s">
+        <v>44</v>
       </c>
       <c r="H7" s="17">
         <v>2</v>
@@ -1211,7 +1208,7 @@
       <c r="AX7" s="1"/>
       <c r="AY7" s="1"/>
     </row>
-    <row r="8" spans="1:51" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="3">
         <v>2</v>
@@ -1224,10 +1221,10 @@
         <v>17</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
-      <c r="G8" s="37" t="s">
-        <v>42</v>
+      <c r="G8" s="28" t="s">
+        <v>39</v>
       </c>
       <c r="H8" s="20">
         <v>1.5</v>
@@ -1278,7 +1275,7 @@
       <c r="AX8" s="1"/>
       <c r="AY8" s="1"/>
     </row>
-    <row r="9" spans="1:51" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="4">
         <v>3</v>
@@ -1288,13 +1285,13 @@
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="G9" s="17" t="s">
         <v>22</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>23</v>
       </c>
       <c r="H9" s="17">
         <v>1.5</v>
@@ -1345,7 +1342,7 @@
       <c r="AX9" s="1"/>
       <c r="AY9" s="1"/>
     </row>
-    <row r="10" spans="1:51" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="5">
         <v>4</v>
@@ -1355,13 +1352,13 @@
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
-      <c r="G10" s="37" t="s">
-        <v>46</v>
+      <c r="G10" s="28" t="s">
+        <v>43</v>
       </c>
       <c r="H10" s="20">
         <v>0.5</v>
@@ -1412,19 +1409,19 @@
       <c r="AX10" s="1"/>
       <c r="AY10" s="1"/>
     </row>
-    <row r="11" spans="1:51" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>18</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H11" s="17">
         <v>1</v>
@@ -1475,19 +1472,19 @@
       <c r="AX11" s="1"/>
       <c r="AY11" s="1"/>
     </row>
-    <row r="12" spans="1:51" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
       <c r="D12" s="6"/>
       <c r="E12" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H12" s="20">
         <v>1.5</v>
@@ -1538,21 +1535,21 @@
       <c r="AX12" s="1"/>
       <c r="AY12" s="1"/>
     </row>
-    <row r="13" spans="1:51" ht="20.149999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:51" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="27"/>
+      <c r="C13" s="30"/>
       <c r="D13" s="6"/>
       <c r="E13" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F13" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="17" t="s">
-        <v>30</v>
+      <c r="G13" s="27" t="s">
+        <v>45</v>
       </c>
       <c r="H13" s="17">
         <v>1</v>
@@ -1603,19 +1600,19 @@
       <c r="AX13" s="1"/>
       <c r="AY13" s="1"/>
     </row>
-    <row r="14" spans="1:51" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
       <c r="D14" s="6"/>
       <c r="E14" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
-      <c r="G14" s="38" t="s">
-        <v>44</v>
+      <c r="G14" s="29" t="s">
+        <v>41</v>
       </c>
       <c r="H14" s="20">
         <v>2</v>
@@ -1666,19 +1663,19 @@
       <c r="AX14" s="1"/>
       <c r="AY14" s="1"/>
     </row>
-    <row r="15" spans="1:51" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
       <c r="D15" s="6"/>
       <c r="E15" s="16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G15" s="26" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H15" s="17">
         <v>2</v>
@@ -1729,21 +1726,21 @@
       <c r="AX15" s="1"/>
       <c r="AY15" s="1"/>
     </row>
-    <row r="16" spans="1:51" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="29"/>
+      <c r="C16" s="32"/>
       <c r="D16" s="6"/>
       <c r="E16" s="19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F16" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="G16" s="20" t="s">
-        <v>35</v>
+      <c r="G16" s="29" t="s">
+        <v>44</v>
       </c>
       <c r="H16" s="20">
         <v>2</v>
@@ -1796,19 +1793,19 @@
       <c r="AX16" s="1"/>
       <c r="AY16" s="1"/>
     </row>
-    <row r="17" spans="1:51" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
       <c r="D17" s="6"/>
       <c r="E17" s="16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
-      <c r="G17" s="36" t="s">
-        <v>45</v>
+      <c r="G17" s="27" t="s">
+        <v>42</v>
       </c>
       <c r="H17" s="17">
         <v>1</v>
@@ -1859,19 +1856,19 @@
       <c r="AX17" s="1"/>
       <c r="AY17" s="1"/>
     </row>
-    <row r="18" spans="1:51" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
       <c r="D18" s="6"/>
       <c r="E18" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H18" s="20">
         <v>1</v>
@@ -1922,19 +1919,19 @@
       <c r="AX18" s="1"/>
       <c r="AY18" s="1"/>
     </row>
-    <row r="19" spans="1:51" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
       <c r="D19" s="6"/>
       <c r="E19" s="16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F19" s="17" t="s">
         <v>18</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H19" s="17">
         <v>2</v>
@@ -1985,10 +1982,10 @@
       <c r="AX19" s="1"/>
       <c r="AY19" s="1"/>
     </row>
-    <row r="20" spans="1:51" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
       <c r="D20" s="6"/>
       <c r="E20" s="19"/>
       <c r="F20" s="20"/>
@@ -2038,10 +2035,10 @@
       <c r="AX20" s="1"/>
       <c r="AY20" s="1"/>
     </row>
-    <row r="21" spans="1:51" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
       <c r="D21" s="6"/>
       <c r="E21" s="16"/>
       <c r="F21" s="17"/>
@@ -2091,10 +2088,10 @@
       <c r="AX21" s="1"/>
       <c r="AY21" s="1"/>
     </row>
-    <row r="22" spans="1:51" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
       <c r="D22" s="6"/>
       <c r="E22" s="19"/>
       <c r="F22" s="20"/>
@@ -2144,10 +2141,10 @@
       <c r="AX22" s="1"/>
       <c r="AY22" s="1"/>
     </row>
-    <row r="23" spans="1:51" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
       <c r="D23" s="6"/>
       <c r="E23" s="16"/>
       <c r="F23" s="17"/>
@@ -2197,10 +2194,10 @@
       <c r="AX23" s="1"/>
       <c r="AY23" s="1"/>
     </row>
-    <row r="24" spans="1:51" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
       <c r="D24" s="6"/>
       <c r="E24" s="19"/>
       <c r="F24" s="20"/>
@@ -2252,7 +2249,7 @@
       <c r="AX24" s="1"/>
       <c r="AY24" s="1"/>
     </row>
-    <row r="25" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -2305,7 +2302,7 @@
       <c r="AX25" s="1"/>
       <c r="AY25" s="1"/>
     </row>
-    <row r="26" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -2358,7 +2355,7 @@
       <c r="AX26" s="1"/>
       <c r="AY26" s="1"/>
     </row>
-    <row r="27" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -2411,7 +2408,7 @@
       <c r="AX27" s="1"/>
       <c r="AY27" s="1"/>
     </row>
-    <row r="28" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -2466,7 +2463,7 @@
       <c r="AX28" s="1"/>
       <c r="AY28" s="1"/>
     </row>
-    <row r="29" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -2519,7 +2516,7 @@
       <c r="AX29" s="1"/>
       <c r="AY29" s="1"/>
     </row>
-    <row r="30" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -2574,7 +2571,7 @@
       <c r="AX30" s="1"/>
       <c r="AY30" s="1"/>
     </row>
-    <row r="31" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -2627,7 +2624,7 @@
       <c r="AX31" s="1"/>
       <c r="AY31" s="1"/>
     </row>
-    <row r="32" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -2680,7 +2677,7 @@
       <c r="AX32" s="1"/>
       <c r="AY32" s="1"/>
     </row>
-    <row r="33" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -2729,7 +2726,7 @@
       <c r="AX33" s="1"/>
       <c r="AY33" s="1"/>
     </row>
-    <row r="34" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -2778,7 +2775,7 @@
       <c r="AX34" s="1"/>
       <c r="AY34" s="1"/>
     </row>
-    <row r="35" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -2827,7 +2824,7 @@
       <c r="AX35" s="1"/>
       <c r="AY35" s="1"/>
     </row>
-    <row r="36" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -2876,7 +2873,7 @@
       <c r="AX36" s="1"/>
       <c r="AY36" s="1"/>
     </row>
-    <row r="37" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -2925,7 +2922,7 @@
       <c r="AX37" s="1"/>
       <c r="AY37" s="1"/>
     </row>
-    <row r="38" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -2974,7 +2971,7 @@
       <c r="AX38" s="1"/>
       <c r="AY38" s="1"/>
     </row>
-    <row r="39" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -3023,7 +3020,7 @@
       <c r="AX39" s="1"/>
       <c r="AY39" s="1"/>
     </row>
-    <row r="40" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -3072,7 +3069,7 @@
       <c r="AX40" s="1"/>
       <c r="AY40" s="1"/>
     </row>
-    <row r="41" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -3121,7 +3118,7 @@
       <c r="AX41" s="1"/>
       <c r="AY41" s="1"/>
     </row>
-    <row r="42" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -3170,7 +3167,7 @@
       <c r="AX42" s="1"/>
       <c r="AY42" s="1"/>
     </row>
-    <row r="43" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -3219,7 +3216,7 @@
       <c r="AX43" s="1"/>
       <c r="AY43" s="1"/>
     </row>
-    <row r="44" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -3268,7 +3265,7 @@
       <c r="AX44" s="1"/>
       <c r="AY44" s="1"/>
     </row>
-    <row r="45" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -3317,7 +3314,7 @@
       <c r="AX45" s="1"/>
       <c r="AY45" s="1"/>
     </row>
-    <row r="46" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -3366,7 +3363,7 @@
       <c r="AX46" s="1"/>
       <c r="AY46" s="1"/>
     </row>
-    <row r="47" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -3415,7 +3412,7 @@
       <c r="AX47" s="1"/>
       <c r="AY47" s="1"/>
     </row>
-    <row r="48" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A48"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -3465,7 +3462,7 @@
       <c r="AX48" s="1"/>
       <c r="AY48" s="1"/>
     </row>
-    <row r="49" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A49"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -3515,7 +3512,7 @@
       <c r="AX49" s="1"/>
       <c r="AY49" s="1"/>
     </row>
-    <row r="50" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A50"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -3565,7 +3562,7 @@
       <c r="AX50" s="1"/>
       <c r="AY50" s="1"/>
     </row>
-    <row r="51" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A51"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -3615,7 +3612,7 @@
       <c r="AX51" s="1"/>
       <c r="AY51" s="1"/>
     </row>
-    <row r="52" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A52"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -3665,7 +3662,7 @@
       <c r="AX52" s="1"/>
       <c r="AY52" s="1"/>
     </row>
-    <row r="53" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A53"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -3715,7 +3712,7 @@
       <c r="AX53" s="1"/>
       <c r="AY53" s="1"/>
     </row>
-    <row r="54" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A54"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -3765,7 +3762,7 @@
       <c r="AX54" s="1"/>
       <c r="AY54" s="1"/>
     </row>
-    <row r="55" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A55"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -3815,7 +3812,7 @@
       <c r="AX55" s="1"/>
       <c r="AY55" s="1"/>
     </row>
-    <row r="56" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A56"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -3865,7 +3862,7 @@
       <c r="AX56" s="1"/>
       <c r="AY56" s="1"/>
     </row>
-    <row r="57" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A57"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -3915,7 +3912,7 @@
       <c r="AX57" s="1"/>
       <c r="AY57" s="1"/>
     </row>
-    <row r="58" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A58"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -3965,7 +3962,7 @@
       <c r="AX58" s="1"/>
       <c r="AY58" s="1"/>
     </row>
-    <row r="59" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A59"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -4015,7 +4012,7 @@
       <c r="AX59" s="1"/>
       <c r="AY59" s="1"/>
     </row>
-    <row r="60" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A60"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -4065,7 +4062,7 @@
       <c r="AX60" s="1"/>
       <c r="AY60" s="1"/>
     </row>
-    <row r="61" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A61"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -4115,7 +4112,7 @@
       <c r="AX61" s="1"/>
       <c r="AY61" s="1"/>
     </row>
-    <row r="62" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A62"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -4167,7 +4164,7 @@
       <c r="AX62" s="1"/>
       <c r="AY62" s="1"/>
     </row>
-    <row r="63" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A63"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -4217,7 +4214,7 @@
       <c r="AX63" s="1"/>
       <c r="AY63" s="1"/>
     </row>
-    <row r="64" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A64"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -4267,7 +4264,7 @@
       <c r="AX64" s="1"/>
       <c r="AY64" s="1"/>
     </row>
-    <row r="65" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A65"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -4317,7 +4314,7 @@
       <c r="AX65" s="1"/>
       <c r="AY65" s="1"/>
     </row>
-    <row r="66" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A66"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -4367,7 +4364,7 @@
       <c r="AX66" s="1"/>
       <c r="AY66" s="1"/>
     </row>
-    <row r="67" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A67"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -4417,7 +4414,7 @@
       <c r="AX67" s="1"/>
       <c r="AY67" s="1"/>
     </row>
-    <row r="68" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A68"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -4467,7 +4464,7 @@
       <c r="AX68" s="1"/>
       <c r="AY68" s="1"/>
     </row>
-    <row r="69" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A69"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -4517,7 +4514,7 @@
       <c r="AX69" s="1"/>
       <c r="AY69" s="1"/>
     </row>
-    <row r="70" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A70"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -4567,7 +4564,7 @@
       <c r="AX70" s="1"/>
       <c r="AY70" s="1"/>
     </row>
-    <row r="71" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A71"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -4617,7 +4614,7 @@
       <c r="AX71" s="1"/>
       <c r="AY71" s="1"/>
     </row>
-    <row r="72" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A72"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -4667,7 +4664,7 @@
       <c r="AX72" s="1"/>
       <c r="AY72" s="1"/>
     </row>
-    <row r="73" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A73"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -4717,7 +4714,7 @@
       <c r="AX73" s="1"/>
       <c r="AY73" s="1"/>
     </row>
-    <row r="74" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A74"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -4767,7 +4764,7 @@
       <c r="AX74" s="1"/>
       <c r="AY74" s="1"/>
     </row>
-    <row r="75" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A75"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -4817,7 +4814,7 @@
       <c r="AX75" s="1"/>
       <c r="AY75" s="1"/>
     </row>
-    <row r="76" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A76"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -4867,7 +4864,7 @@
       <c r="AX76" s="1"/>
       <c r="AY76" s="1"/>
     </row>
-    <row r="77" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A77"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -4917,7 +4914,7 @@
       <c r="AX77" s="1"/>
       <c r="AY77" s="1"/>
     </row>
-    <row r="78" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A78"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -4967,7 +4964,7 @@
       <c r="AX78" s="1"/>
       <c r="AY78" s="1"/>
     </row>
-    <row r="79" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A79"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -5017,7 +5014,7 @@
       <c r="AX79" s="1"/>
       <c r="AY79" s="1"/>
     </row>
-    <row r="80" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A80"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -5067,7 +5064,7 @@
       <c r="AX80" s="1"/>
       <c r="AY80" s="1"/>
     </row>
-    <row r="81" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A81"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -5117,7 +5114,7 @@
       <c r="AX81" s="1"/>
       <c r="AY81" s="1"/>
     </row>
-    <row r="82" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A82"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -5167,7 +5164,7 @@
       <c r="AX82" s="1"/>
       <c r="AY82" s="1"/>
     </row>
-    <row r="83" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A83"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -5217,7 +5214,7 @@
       <c r="AX83" s="1"/>
       <c r="AY83" s="1"/>
     </row>
-    <row r="84" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A84"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -5267,7 +5264,7 @@
       <c r="AX84" s="1"/>
       <c r="AY84" s="1"/>
     </row>
-    <row r="85" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A85"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -5317,7 +5314,7 @@
       <c r="AX85" s="1"/>
       <c r="AY85" s="1"/>
     </row>
-    <row r="86" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A86"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -5367,7 +5364,7 @@
       <c r="AX86" s="1"/>
       <c r="AY86" s="1"/>
     </row>
-    <row r="87" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A87"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -5417,7 +5414,7 @@
       <c r="AX87" s="1"/>
       <c r="AY87" s="1"/>
     </row>
-    <row r="88" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A88"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -5467,7 +5464,7 @@
       <c r="AX88" s="1"/>
       <c r="AY88" s="1"/>
     </row>
-    <row r="89" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A89"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -5517,7 +5514,7 @@
       <c r="AX89" s="1"/>
       <c r="AY89" s="1"/>
     </row>
-    <row r="90" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A90"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -5567,7 +5564,7 @@
       <c r="AX90" s="1"/>
       <c r="AY90" s="1"/>
     </row>
-    <row r="91" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A91"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -5617,7 +5614,7 @@
       <c r="AX91" s="1"/>
       <c r="AY91" s="1"/>
     </row>
-    <row r="92" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A92"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -5667,7 +5664,7 @@
       <c r="AX92" s="1"/>
       <c r="AY92" s="1"/>
     </row>
-    <row r="93" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A93"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -5717,7 +5714,7 @@
       <c r="AX93" s="1"/>
       <c r="AY93" s="1"/>
     </row>
-    <row r="94" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A94"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -5767,7 +5764,7 @@
       <c r="AX94" s="1"/>
       <c r="AY94" s="1"/>
     </row>
-    <row r="95" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A95"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -5817,7 +5814,7 @@
       <c r="AX95" s="1"/>
       <c r="AY95" s="1"/>
     </row>
-    <row r="96" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A96"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -5867,7 +5864,7 @@
       <c r="AX96" s="1"/>
       <c r="AY96" s="1"/>
     </row>
-    <row r="97" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A97"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -5917,7 +5914,7 @@
       <c r="AX97" s="1"/>
       <c r="AY97" s="1"/>
     </row>
-    <row r="98" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A98"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -5967,7 +5964,7 @@
       <c r="AX98" s="1"/>
       <c r="AY98" s="1"/>
     </row>
-    <row r="99" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A99"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -6017,7 +6014,7 @@
       <c r="AX99" s="1"/>
       <c r="AY99" s="1"/>
     </row>
-    <row r="100" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A100"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -6067,7 +6064,7 @@
       <c r="AX100" s="1"/>
       <c r="AY100" s="1"/>
     </row>
-    <row r="101" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A101"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -6117,7 +6114,7 @@
       <c r="AX101" s="1"/>
       <c r="AY101" s="1"/>
     </row>
-    <row r="102" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A102"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -6167,7 +6164,7 @@
       <c r="AX102" s="1"/>
       <c r="AY102" s="1"/>
     </row>
-    <row r="103" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A103"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -6217,7 +6214,7 @@
       <c r="AX103" s="1"/>
       <c r="AY103" s="1"/>
     </row>
-    <row r="104" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A104"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -6267,7 +6264,7 @@
       <c r="AX104" s="1"/>
       <c r="AY104" s="1"/>
     </row>
-    <row r="105" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A105"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -6317,7 +6314,7 @@
       <c r="AX105" s="1"/>
       <c r="AY105" s="1"/>
     </row>
-    <row r="106" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A106"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -6367,7 +6364,7 @@
       <c r="AX106" s="1"/>
       <c r="AY106" s="1"/>
     </row>
-    <row r="107" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A107"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -6417,7 +6414,7 @@
       <c r="AX107" s="1"/>
       <c r="AY107" s="1"/>
     </row>
-    <row r="108" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A108"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -6467,7 +6464,7 @@
       <c r="AX108" s="1"/>
       <c r="AY108" s="1"/>
     </row>
-    <row r="109" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A109"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -6517,7 +6514,7 @@
       <c r="AX109" s="1"/>
       <c r="AY109" s="1"/>
     </row>
-    <row r="110" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A110"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -6567,7 +6564,7 @@
       <c r="AX110" s="1"/>
       <c r="AY110" s="1"/>
     </row>
-    <row r="111" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A111"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -6617,7 +6614,7 @@
       <c r="AX111" s="1"/>
       <c r="AY111" s="1"/>
     </row>
-    <row r="112" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A112"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -6667,7 +6664,7 @@
       <c r="AX112" s="1"/>
       <c r="AY112" s="1"/>
     </row>
-    <row r="113" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A113"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -6717,7 +6714,7 @@
       <c r="AX113" s="1"/>
       <c r="AY113" s="1"/>
     </row>
-    <row r="114" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A114"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -6767,7 +6764,7 @@
       <c r="AX114" s="1"/>
       <c r="AY114" s="1"/>
     </row>
-    <row r="115" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A115"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -6817,7 +6814,7 @@
       <c r="AX115" s="1"/>
       <c r="AY115" s="1"/>
     </row>
-    <row r="116" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A116"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -6867,7 +6864,7 @@
       <c r="AX116" s="1"/>
       <c r="AY116" s="1"/>
     </row>
-    <row r="117" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A117"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -6917,7 +6914,7 @@
       <c r="AX117" s="1"/>
       <c r="AY117" s="1"/>
     </row>
-    <row r="118" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A118"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -6967,7 +6964,7 @@
       <c r="AX118" s="1"/>
       <c r="AY118" s="1"/>
     </row>
-    <row r="119" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A119"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -7017,7 +7014,7 @@
       <c r="AX119" s="1"/>
       <c r="AY119" s="1"/>
     </row>
-    <row r="120" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A120"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -7067,7 +7064,7 @@
       <c r="AX120" s="1"/>
       <c r="AY120" s="1"/>
     </row>
-    <row r="121" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A121"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -7117,7 +7114,7 @@
       <c r="AX121" s="1"/>
       <c r="AY121" s="1"/>
     </row>
-    <row r="122" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A122"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -7167,7 +7164,7 @@
       <c r="AX122" s="1"/>
       <c r="AY122" s="1"/>
     </row>
-    <row r="123" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A123"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -7217,7 +7214,7 @@
       <c r="AX123" s="1"/>
       <c r="AY123" s="1"/>
     </row>
-    <row r="124" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A124"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -7267,7 +7264,7 @@
       <c r="AX124" s="1"/>
       <c r="AY124" s="1"/>
     </row>
-    <row r="125" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A125"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -7317,7 +7314,7 @@
       <c r="AX125" s="1"/>
       <c r="AY125" s="1"/>
     </row>
-    <row r="126" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A126"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -7367,7 +7364,7 @@
       <c r="AX126" s="1"/>
       <c r="AY126" s="1"/>
     </row>
-    <row r="127" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A127"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -7417,7 +7414,7 @@
       <c r="AX127" s="1"/>
       <c r="AY127" s="1"/>
     </row>
-    <row r="128" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A128"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -7467,7 +7464,7 @@
       <c r="AX128" s="1"/>
       <c r="AY128" s="1"/>
     </row>
-    <row r="129" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A129"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -7517,7 +7514,7 @@
       <c r="AX129" s="1"/>
       <c r="AY129" s="1"/>
     </row>
-    <row r="130" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A130"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -7567,7 +7564,7 @@
       <c r="AX130" s="1"/>
       <c r="AY130" s="1"/>
     </row>
-    <row r="131" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A131"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -7617,7 +7614,7 @@
       <c r="AX131" s="1"/>
       <c r="AY131" s="1"/>
     </row>
-    <row r="132" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A132"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -7667,7 +7664,7 @@
       <c r="AX132" s="1"/>
       <c r="AY132" s="1"/>
     </row>
-    <row r="133" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A133"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -7717,7 +7714,7 @@
       <c r="AX133" s="1"/>
       <c r="AY133" s="1"/>
     </row>
-    <row r="134" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A134"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -7767,7 +7764,7 @@
       <c r="AX134" s="1"/>
       <c r="AY134" s="1"/>
     </row>
-    <row r="135" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A135"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -7817,7 +7814,7 @@
       <c r="AX135" s="1"/>
       <c r="AY135" s="1"/>
     </row>
-    <row r="136" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A136"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -7867,7 +7864,7 @@
       <c r="AX136" s="1"/>
       <c r="AY136" s="1"/>
     </row>
-    <row r="137" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A137"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -7917,7 +7914,7 @@
       <c r="AX137" s="1"/>
       <c r="AY137" s="1"/>
     </row>
-    <row r="138" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A138"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -7967,7 +7964,7 @@
       <c r="AX138" s="1"/>
       <c r="AY138" s="1"/>
     </row>
-    <row r="139" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A139"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -8017,7 +8014,7 @@
       <c r="AX139" s="1"/>
       <c r="AY139" s="1"/>
     </row>
-    <row r="140" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A140"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -8067,7 +8064,7 @@
       <c r="AX140" s="1"/>
       <c r="AY140" s="1"/>
     </row>
-    <row r="141" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A141"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -8117,7 +8114,7 @@
       <c r="AX141" s="1"/>
       <c r="AY141" s="1"/>
     </row>
-    <row r="142" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A142"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -8167,7 +8164,7 @@
       <c r="AX142" s="1"/>
       <c r="AY142" s="1"/>
     </row>
-    <row r="143" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A143"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -8217,7 +8214,7 @@
       <c r="AX143" s="1"/>
       <c r="AY143" s="1"/>
     </row>
-    <row r="144" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A144"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -8267,7 +8264,7 @@
       <c r="AX144" s="1"/>
       <c r="AY144" s="1"/>
     </row>
-    <row r="145" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A145"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -8317,7 +8314,7 @@
       <c r="AX145" s="1"/>
       <c r="AY145" s="1"/>
     </row>
-    <row r="146" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A146"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -8367,7 +8364,7 @@
       <c r="AX146" s="1"/>
       <c r="AY146" s="1"/>
     </row>
-    <row r="147" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A147"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -8417,7 +8414,7 @@
       <c r="AX147" s="1"/>
       <c r="AY147" s="1"/>
     </row>
-    <row r="148" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A148"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -8467,7 +8464,7 @@
       <c r="AX148" s="1"/>
       <c r="AY148" s="1"/>
     </row>
-    <row r="149" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A149"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -8517,7 +8514,7 @@
       <c r="AX149" s="1"/>
       <c r="AY149" s="1"/>
     </row>
-    <row r="150" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A150"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -8567,7 +8564,7 @@
       <c r="AX150" s="1"/>
       <c r="AY150" s="1"/>
     </row>
-    <row r="151" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A151"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -8617,7 +8614,7 @@
       <c r="AX151" s="1"/>
       <c r="AY151" s="1"/>
     </row>
-    <row r="152" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A152"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -8667,7 +8664,7 @@
       <c r="AX152" s="1"/>
       <c r="AY152" s="1"/>
     </row>
-    <row r="153" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A153"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -8717,7 +8714,7 @@
       <c r="AX153" s="1"/>
       <c r="AY153" s="1"/>
     </row>
-    <row r="154" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A154"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -8767,7 +8764,7 @@
       <c r="AX154" s="1"/>
       <c r="AY154" s="1"/>
     </row>
-    <row r="155" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A155"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -8817,7 +8814,7 @@
       <c r="AX155" s="1"/>
       <c r="AY155" s="1"/>
     </row>
-    <row r="156" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A156"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -8867,7 +8864,7 @@
       <c r="AX156" s="1"/>
       <c r="AY156" s="1"/>
     </row>
-    <row r="157" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A157"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -8917,7 +8914,7 @@
       <c r="AX157" s="1"/>
       <c r="AY157" s="1"/>
     </row>
-    <row r="158" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A158"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -8967,7 +8964,7 @@
       <c r="AX158" s="1"/>
       <c r="AY158" s="1"/>
     </row>
-    <row r="159" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A159"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -9017,7 +9014,7 @@
       <c r="AX159" s="1"/>
       <c r="AY159" s="1"/>
     </row>
-    <row r="160" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A160"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -9067,7 +9064,7 @@
       <c r="AX160" s="1"/>
       <c r="AY160" s="1"/>
     </row>
-    <row r="161" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A161"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -9117,7 +9114,7 @@
       <c r="AX161" s="1"/>
       <c r="AY161" s="1"/>
     </row>
-    <row r="162" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A162"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -9167,7 +9164,7 @@
       <c r="AX162" s="1"/>
       <c r="AY162" s="1"/>
     </row>
-    <row r="163" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A163"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -9217,7 +9214,7 @@
       <c r="AX163" s="1"/>
       <c r="AY163" s="1"/>
     </row>
-    <row r="164" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A164"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -9267,7 +9264,7 @@
       <c r="AX164" s="1"/>
       <c r="AY164" s="1"/>
     </row>
-    <row r="165" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A165"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -9317,7 +9314,7 @@
       <c r="AX165" s="1"/>
       <c r="AY165" s="1"/>
     </row>
-    <row r="166" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A166"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -9367,7 +9364,7 @@
       <c r="AX166" s="1"/>
       <c r="AY166" s="1"/>
     </row>
-    <row r="167" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A167"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -9417,7 +9414,7 @@
       <c r="AX167" s="1"/>
       <c r="AY167" s="1"/>
     </row>
-    <row r="168" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A168"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -9467,7 +9464,7 @@
       <c r="AX168" s="1"/>
       <c r="AY168" s="1"/>
     </row>
-    <row r="169" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A169"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -9517,7 +9514,7 @@
       <c r="AX169" s="1"/>
       <c r="AY169" s="1"/>
     </row>
-    <row r="170" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A170"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -9567,7 +9564,7 @@
       <c r="AX170" s="1"/>
       <c r="AY170" s="1"/>
     </row>
-    <row r="171" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A171"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -9617,7 +9614,7 @@
       <c r="AX171" s="1"/>
       <c r="AY171" s="1"/>
     </row>
-    <row r="172" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A172"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -9667,7 +9664,7 @@
       <c r="AX172" s="1"/>
       <c r="AY172" s="1"/>
     </row>
-    <row r="173" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A173"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -9717,7 +9714,7 @@
       <c r="AX173" s="1"/>
       <c r="AY173" s="1"/>
     </row>
-    <row r="174" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A174"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -9767,7 +9764,7 @@
       <c r="AX174" s="1"/>
       <c r="AY174" s="1"/>
     </row>
-    <row r="175" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A175"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -9817,7 +9814,7 @@
       <c r="AX175" s="1"/>
       <c r="AY175" s="1"/>
     </row>
-    <row r="176" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A176"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -9867,7 +9864,7 @@
       <c r="AX176" s="1"/>
       <c r="AY176" s="1"/>
     </row>
-    <row r="177" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A177"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -9917,7 +9914,7 @@
       <c r="AX177" s="1"/>
       <c r="AY177" s="1"/>
     </row>
-    <row r="178" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A178"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -9967,7 +9964,7 @@
       <c r="AX178" s="1"/>
       <c r="AY178" s="1"/>
     </row>
-    <row r="179" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A179"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -10017,7 +10014,7 @@
       <c r="AX179" s="1"/>
       <c r="AY179" s="1"/>
     </row>
-    <row r="180" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A180"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -10067,7 +10064,7 @@
       <c r="AX180" s="1"/>
       <c r="AY180" s="1"/>
     </row>
-    <row r="181" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A181"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -10117,7 +10114,7 @@
       <c r="AX181" s="1"/>
       <c r="AY181" s="1"/>
     </row>
-    <row r="182" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A182"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -10167,7 +10164,7 @@
       <c r="AX182" s="1"/>
       <c r="AY182" s="1"/>
     </row>
-    <row r="183" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A183"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -10217,7 +10214,7 @@
       <c r="AX183" s="1"/>
       <c r="AY183" s="1"/>
     </row>
-    <row r="184" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A184"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -10267,7 +10264,7 @@
       <c r="AX184" s="1"/>
       <c r="AY184" s="1"/>
     </row>
-    <row r="185" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A185"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -10317,7 +10314,7 @@
       <c r="AX185" s="1"/>
       <c r="AY185" s="1"/>
     </row>
-    <row r="186" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A186"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -10367,7 +10364,7 @@
       <c r="AX186" s="1"/>
       <c r="AY186" s="1"/>
     </row>
-    <row r="187" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A187"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -10417,7 +10414,7 @@
       <c r="AX187" s="1"/>
       <c r="AY187" s="1"/>
     </row>
-    <row r="188" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A188"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -10467,7 +10464,7 @@
       <c r="AX188" s="1"/>
       <c r="AY188" s="1"/>
     </row>
-    <row r="189" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A189"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -10517,7 +10514,7 @@
       <c r="AX189" s="1"/>
       <c r="AY189" s="1"/>
     </row>
-    <row r="190" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A190"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -10567,7 +10564,7 @@
       <c r="AX190" s="1"/>
       <c r="AY190" s="1"/>
     </row>
-    <row r="191" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A191"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -10617,7 +10614,7 @@
       <c r="AX191" s="1"/>
       <c r="AY191" s="1"/>
     </row>
-    <row r="192" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A192"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -10667,7 +10664,7 @@
       <c r="AX192" s="1"/>
       <c r="AY192" s="1"/>
     </row>
-    <row r="193" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A193"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -10717,7 +10714,7 @@
       <c r="AX193" s="1"/>
       <c r="AY193" s="1"/>
     </row>
-    <row r="194" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A194"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -10767,7 +10764,7 @@
       <c r="AX194" s="1"/>
       <c r="AY194" s="1"/>
     </row>
-    <row r="195" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A195"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -10817,7 +10814,7 @@
       <c r="AX195" s="1"/>
       <c r="AY195" s="1"/>
     </row>
-    <row r="196" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A196"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -10867,7 +10864,7 @@
       <c r="AX196" s="1"/>
       <c r="AY196" s="1"/>
     </row>
-    <row r="197" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A197"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -10917,7 +10914,7 @@
       <c r="AX197" s="1"/>
       <c r="AY197" s="1"/>
     </row>
-    <row r="198" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A198"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -10967,7 +10964,7 @@
       <c r="AX198" s="1"/>
       <c r="AY198" s="1"/>
     </row>
-    <row r="199" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A199"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -11017,7 +11014,7 @@
       <c r="AX199" s="1"/>
       <c r="AY199" s="1"/>
     </row>
-    <row r="200" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A200"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
@@ -11067,7 +11064,7 @@
       <c r="AX200" s="1"/>
       <c r="AY200" s="1"/>
     </row>
-    <row r="201" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A201"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
@@ -11117,7 +11114,7 @@
       <c r="AX201" s="1"/>
       <c r="AY201" s="1"/>
     </row>
-    <row r="202" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A202"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
@@ -11167,7 +11164,7 @@
       <c r="AX202" s="1"/>
       <c r="AY202" s="1"/>
     </row>
-    <row r="203" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A203"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
@@ -11217,7 +11214,7 @@
       <c r="AX203" s="1"/>
       <c r="AY203" s="1"/>
     </row>
-    <row r="204" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A204"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
@@ -11267,7 +11264,7 @@
       <c r="AX204" s="1"/>
       <c r="AY204" s="1"/>
     </row>
-    <row r="205" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A205"/>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
@@ -11317,7 +11314,7 @@
       <c r="AX205" s="1"/>
       <c r="AY205" s="1"/>
     </row>
-    <row r="206" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A206"/>
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
@@ -11367,7 +11364,7 @@
       <c r="AX206" s="1"/>
       <c r="AY206" s="1"/>
     </row>
-    <row r="207" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A207"/>
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
@@ -11417,7 +11414,7 @@
       <c r="AX207" s="1"/>
       <c r="AY207" s="1"/>
     </row>
-    <row r="208" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A208"/>
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
@@ -11467,7 +11464,7 @@
       <c r="AX208" s="1"/>
       <c r="AY208" s="1"/>
     </row>
-    <row r="209" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A209"/>
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
@@ -11517,7 +11514,7 @@
       <c r="AX209" s="1"/>
       <c r="AY209" s="1"/>
     </row>
-    <row r="210" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A210"/>
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
@@ -11567,7 +11564,7 @@
       <c r="AX210" s="1"/>
       <c r="AY210" s="1"/>
     </row>
-    <row r="211" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A211"/>
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
@@ -11617,7 +11614,7 @@
       <c r="AX211" s="1"/>
       <c r="AY211" s="1"/>
     </row>
-    <row r="212" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A212"/>
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
@@ -11667,7 +11664,7 @@
       <c r="AX212" s="1"/>
       <c r="AY212" s="1"/>
     </row>
-    <row r="213" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A213"/>
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
@@ -11717,7 +11714,7 @@
       <c r="AX213" s="1"/>
       <c r="AY213" s="1"/>
     </row>
-    <row r="214" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A214"/>
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
@@ -11767,7 +11764,7 @@
       <c r="AX214" s="1"/>
       <c r="AY214" s="1"/>
     </row>
-    <row r="215" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A215"/>
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
@@ -11817,7 +11814,7 @@
       <c r="AX215" s="1"/>
       <c r="AY215" s="1"/>
     </row>
-    <row r="216" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A216"/>
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
@@ -11867,7 +11864,7 @@
       <c r="AX216" s="1"/>
       <c r="AY216" s="1"/>
     </row>
-    <row r="217" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A217"/>
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
@@ -11917,7 +11914,7 @@
       <c r="AX217" s="1"/>
       <c r="AY217" s="1"/>
     </row>
-    <row r="218" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A218"/>
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
@@ -11967,7 +11964,7 @@
       <c r="AX218" s="1"/>
       <c r="AY218" s="1"/>
     </row>
-    <row r="219" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A219"/>
       <c r="B219" s="1"/>
       <c r="C219" s="1"/>
@@ -12017,7 +12014,7 @@
       <c r="AX219" s="1"/>
       <c r="AY219" s="1"/>
     </row>
-    <row r="220" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A220"/>
       <c r="B220" s="1"/>
       <c r="C220" s="1"/>
@@ -12067,7 +12064,7 @@
       <c r="AX220" s="1"/>
       <c r="AY220" s="1"/>
     </row>
-    <row r="221" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A221"/>
       <c r="B221" s="1"/>
       <c r="C221" s="1"/>
@@ -12117,7 +12114,7 @@
       <c r="AX221" s="1"/>
       <c r="AY221" s="1"/>
     </row>
-    <row r="222" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A222"/>
       <c r="B222" s="1"/>
       <c r="C222" s="1"/>
@@ -12167,7 +12164,7 @@
       <c r="AX222" s="1"/>
       <c r="AY222" s="1"/>
     </row>
-    <row r="223" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A223"/>
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
@@ -12217,7 +12214,7 @@
       <c r="AX223" s="1"/>
       <c r="AY223" s="1"/>
     </row>
-    <row r="224" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A224"/>
       <c r="B224" s="1"/>
       <c r="C224" s="1"/>
@@ -12267,7 +12264,7 @@
       <c r="AX224" s="1"/>
       <c r="AY224" s="1"/>
     </row>
-    <row r="225" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A225"/>
       <c r="B225" s="1"/>
       <c r="C225" s="1"/>
@@ -12317,7 +12314,7 @@
       <c r="AX225" s="1"/>
       <c r="AY225" s="1"/>
     </row>
-    <row r="226" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A226"/>
       <c r="B226" s="1"/>
       <c r="C226" s="1"/>
@@ -12367,7 +12364,7 @@
       <c r="AX226" s="1"/>
       <c r="AY226" s="1"/>
     </row>
-    <row r="227" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A227"/>
       <c r="B227" s="1"/>
       <c r="C227" s="1"/>
@@ -12417,7 +12414,7 @@
       <c r="AX227" s="1"/>
       <c r="AY227" s="1"/>
     </row>
-    <row r="228" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A228"/>
       <c r="B228" s="1"/>
       <c r="C228" s="1"/>
@@ -12467,7 +12464,7 @@
       <c r="AX228" s="1"/>
       <c r="AY228" s="1"/>
     </row>
-    <row r="229" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A229"/>
       <c r="B229" s="1"/>
       <c r="C229" s="1"/>
@@ -12517,7 +12514,7 @@
       <c r="AX229" s="1"/>
       <c r="AY229" s="1"/>
     </row>
-    <row r="230" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A230"/>
       <c r="B230" s="1"/>
       <c r="C230" s="1"/>
@@ -12567,7 +12564,7 @@
       <c r="AX230" s="1"/>
       <c r="AY230" s="1"/>
     </row>
-    <row r="231" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A231"/>
       <c r="B231" s="1"/>
       <c r="C231" s="1"/>
@@ -12617,7 +12614,7 @@
       <c r="AX231" s="1"/>
       <c r="AY231" s="1"/>
     </row>
-    <row r="232" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A232"/>
       <c r="B232" s="1"/>
       <c r="C232" s="1"/>
@@ -12667,7 +12664,7 @@
       <c r="AX232" s="1"/>
       <c r="AY232" s="1"/>
     </row>
-    <row r="233" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A233"/>
       <c r="B233" s="1"/>
       <c r="C233" s="1"/>
@@ -12717,7 +12714,7 @@
       <c r="AX233" s="1"/>
       <c r="AY233" s="1"/>
     </row>
-    <row r="234" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A234"/>
       <c r="B234" s="1"/>
       <c r="C234" s="1"/>
@@ -12767,7 +12764,7 @@
       <c r="AX234" s="1"/>
       <c r="AY234" s="1"/>
     </row>
-    <row r="235" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A235"/>
       <c r="B235" s="1"/>
       <c r="C235" s="1"/>
@@ -12817,7 +12814,7 @@
       <c r="AX235" s="1"/>
       <c r="AY235" s="1"/>
     </row>
-    <row r="236" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A236"/>
       <c r="B236" s="1"/>
       <c r="C236" s="1"/>
@@ -12867,7 +12864,7 @@
       <c r="AX236" s="1"/>
       <c r="AY236" s="1"/>
     </row>
-    <row r="237" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A237"/>
       <c r="B237" s="1"/>
       <c r="C237" s="1"/>
@@ -12917,7 +12914,7 @@
       <c r="AX237" s="1"/>
       <c r="AY237" s="1"/>
     </row>
-    <row r="238" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A238"/>
       <c r="B238" s="1"/>
       <c r="C238" s="1"/>
@@ -12967,7 +12964,7 @@
       <c r="AX238" s="1"/>
       <c r="AY238" s="1"/>
     </row>
-    <row r="239" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A239"/>
       <c r="B239" s="1"/>
       <c r="C239" s="1"/>
@@ -13017,7 +13014,7 @@
       <c r="AX239" s="1"/>
       <c r="AY239" s="1"/>
     </row>
-    <row r="240" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A240"/>
       <c r="B240" s="1"/>
       <c r="C240" s="1"/>
@@ -13067,7 +13064,7 @@
       <c r="AX240" s="1"/>
       <c r="AY240" s="1"/>
     </row>
-    <row r="241" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A241"/>
       <c r="B241" s="1"/>
       <c r="C241" s="1"/>
@@ -13117,7 +13114,7 @@
       <c r="AX241" s="1"/>
       <c r="AY241" s="1"/>
     </row>
-    <row r="242" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A242"/>
       <c r="B242" s="1"/>
       <c r="C242" s="1"/>
@@ -13167,7 +13164,7 @@
       <c r="AX242" s="1"/>
       <c r="AY242" s="1"/>
     </row>
-    <row r="243" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A243"/>
       <c r="B243" s="1"/>
       <c r="C243" s="1"/>
@@ -13217,7 +13214,7 @@
       <c r="AX243" s="1"/>
       <c r="AY243" s="1"/>
     </row>
-    <row r="244" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A244"/>
       <c r="B244" s="1"/>
       <c r="C244" s="1"/>
@@ -13267,7 +13264,7 @@
       <c r="AX244" s="1"/>
       <c r="AY244" s="1"/>
     </row>
-    <row r="245" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A245"/>
       <c r="B245" s="1"/>
       <c r="C245" s="1"/>
@@ -13317,7 +13314,7 @@
       <c r="AX245" s="1"/>
       <c r="AY245" s="1"/>
     </row>
-    <row r="246" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A246"/>
       <c r="B246" s="1"/>
       <c r="C246" s="1"/>
@@ -13367,7 +13364,7 @@
       <c r="AX246" s="1"/>
       <c r="AY246" s="1"/>
     </row>
-    <row r="247" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A247"/>
       <c r="B247" s="1"/>
       <c r="C247" s="1"/>
@@ -13417,7 +13414,7 @@
       <c r="AX247" s="1"/>
       <c r="AY247" s="1"/>
     </row>
-    <row r="248" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A248"/>
       <c r="B248" s="1"/>
       <c r="C248" s="1"/>
@@ -13467,7 +13464,7 @@
       <c r="AX248" s="1"/>
       <c r="AY248" s="1"/>
     </row>
-    <row r="249" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A249"/>
       <c r="B249" s="1"/>
       <c r="C249" s="1"/>
@@ -13517,7 +13514,7 @@
       <c r="AX249" s="1"/>
       <c r="AY249" s="1"/>
     </row>
-    <row r="250" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A250"/>
       <c r="B250" s="1"/>
       <c r="C250" s="1"/>
@@ -13567,7 +13564,7 @@
       <c r="AX250" s="1"/>
       <c r="AY250" s="1"/>
     </row>
-    <row r="251" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A251"/>
       <c r="B251" s="1"/>
       <c r="C251" s="1"/>
@@ -13617,7 +13614,7 @@
       <c r="AX251" s="1"/>
       <c r="AY251" s="1"/>
     </row>
-    <row r="252" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A252"/>
       <c r="B252" s="1"/>
       <c r="C252" s="1"/>
@@ -13667,7 +13664,7 @@
       <c r="AX252" s="1"/>
       <c r="AY252" s="1"/>
     </row>
-    <row r="253" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A253"/>
       <c r="B253" s="1"/>
       <c r="C253" s="1"/>
@@ -13717,7 +13714,7 @@
       <c r="AX253" s="1"/>
       <c r="AY253" s="1"/>
     </row>
-    <row r="254" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A254"/>
       <c r="B254" s="1"/>
       <c r="C254" s="1"/>
@@ -13767,7 +13764,7 @@
       <c r="AX254" s="1"/>
       <c r="AY254" s="1"/>
     </row>
-    <row r="255" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A255"/>
       <c r="B255" s="1"/>
       <c r="C255" s="1"/>
@@ -13817,7 +13814,7 @@
       <c r="AX255" s="1"/>
       <c r="AY255" s="1"/>
     </row>
-    <row r="256" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A256"/>
       <c r="B256" s="1"/>
       <c r="C256" s="1"/>
@@ -13867,7 +13864,7 @@
       <c r="AX256" s="1"/>
       <c r="AY256" s="1"/>
     </row>
-    <row r="257" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A257"/>
       <c r="B257" s="1"/>
       <c r="C257" s="1"/>
@@ -13917,7 +13914,7 @@
       <c r="AX257" s="1"/>
       <c r="AY257" s="1"/>
     </row>
-    <row r="258" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A258"/>
       <c r="B258" s="1"/>
       <c r="C258" s="1"/>
@@ -13967,7 +13964,7 @@
       <c r="AX258" s="1"/>
       <c r="AY258" s="1"/>
     </row>
-    <row r="259" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A259"/>
       <c r="B259" s="1"/>
       <c r="C259" s="1"/>
@@ -14017,7 +14014,7 @@
       <c r="AX259" s="1"/>
       <c r="AY259" s="1"/>
     </row>
-    <row r="260" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A260"/>
       <c r="B260" s="1"/>
       <c r="C260" s="1"/>
@@ -14067,7 +14064,7 @@
       <c r="AX260" s="1"/>
       <c r="AY260" s="1"/>
     </row>
-    <row r="261" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A261"/>
       <c r="B261" s="1"/>
       <c r="C261" s="1"/>
@@ -14117,7 +14114,7 @@
       <c r="AX261" s="1"/>
       <c r="AY261" s="1"/>
     </row>
-    <row r="262" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A262"/>
       <c r="B262" s="1"/>
       <c r="C262" s="1"/>
@@ -14167,7 +14164,7 @@
       <c r="AX262" s="1"/>
       <c r="AY262" s="1"/>
     </row>
-    <row r="263" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A263"/>
       <c r="B263" s="1"/>
       <c r="C263" s="1"/>
@@ -14217,7 +14214,7 @@
       <c r="AX263" s="1"/>
       <c r="AY263" s="1"/>
     </row>
-    <row r="264" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A264"/>
       <c r="B264" s="1"/>
       <c r="C264" s="1"/>
@@ -14267,7 +14264,7 @@
       <c r="AX264" s="1"/>
       <c r="AY264" s="1"/>
     </row>
-    <row r="265" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A265"/>
       <c r="B265" s="1"/>
       <c r="C265" s="1"/>
@@ -14317,7 +14314,7 @@
       <c r="AX265" s="1"/>
       <c r="AY265" s="1"/>
     </row>
-    <row r="266" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A266"/>
       <c r="B266" s="1"/>
       <c r="C266" s="1"/>
@@ -14367,7 +14364,7 @@
       <c r="AX266" s="1"/>
       <c r="AY266" s="1"/>
     </row>
-    <row r="267" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A267"/>
       <c r="B267" s="1"/>
       <c r="C267" s="1"/>
@@ -14417,7 +14414,7 @@
       <c r="AX267" s="1"/>
       <c r="AY267" s="1"/>
     </row>
-    <row r="268" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A268"/>
       <c r="B268" s="1"/>
       <c r="C268" s="1"/>
@@ -14467,7 +14464,7 @@
       <c r="AX268" s="1"/>
       <c r="AY268" s="1"/>
     </row>
-    <row r="269" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A269"/>
       <c r="B269" s="1"/>
       <c r="C269" s="1"/>
@@ -14517,7 +14514,7 @@
       <c r="AX269" s="1"/>
       <c r="AY269" s="1"/>
     </row>
-    <row r="270" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A270"/>
       <c r="B270" s="1"/>
       <c r="C270" s="1"/>
@@ -14567,7 +14564,7 @@
       <c r="AX270" s="1"/>
       <c r="AY270" s="1"/>
     </row>
-    <row r="271" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A271"/>
       <c r="B271" s="1"/>
       <c r="C271" s="1"/>
@@ -14617,7 +14614,7 @@
       <c r="AX271" s="1"/>
       <c r="AY271" s="1"/>
     </row>
-    <row r="272" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A272"/>
       <c r="B272" s="1"/>
       <c r="C272" s="1"/>
@@ -14667,7 +14664,7 @@
       <c r="AX272" s="1"/>
       <c r="AY272" s="1"/>
     </row>
-    <row r="273" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A273"/>
       <c r="B273" s="1"/>
       <c r="C273" s="1"/>
@@ -14717,7 +14714,7 @@
       <c r="AX273" s="1"/>
       <c r="AY273" s="1"/>
     </row>
-    <row r="274" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A274"/>
       <c r="B274" s="1"/>
       <c r="C274" s="1"/>
@@ -14767,7 +14764,7 @@
       <c r="AX274" s="1"/>
       <c r="AY274" s="1"/>
     </row>
-    <row r="275" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A275"/>
       <c r="B275" s="1"/>
       <c r="C275" s="1"/>
@@ -14817,7 +14814,7 @@
       <c r="AX275" s="1"/>
       <c r="AY275" s="1"/>
     </row>
-    <row r="276" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A276"/>
       <c r="B276" s="1"/>
       <c r="C276" s="1"/>
@@ -14867,7 +14864,7 @@
       <c r="AX276" s="1"/>
       <c r="AY276" s="1"/>
     </row>
-    <row r="277" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A277"/>
       <c r="B277" s="1"/>
       <c r="C277" s="1"/>
@@ -14917,7 +14914,7 @@
       <c r="AX277" s="1"/>
       <c r="AY277" s="1"/>
     </row>
-    <row r="278" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A278"/>
       <c r="B278" s="1"/>
       <c r="C278" s="1"/>
@@ -14967,7 +14964,7 @@
       <c r="AX278" s="1"/>
       <c r="AY278" s="1"/>
     </row>
-    <row r="279" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A279"/>
       <c r="B279" s="1"/>
       <c r="C279" s="1"/>
@@ -15017,7 +15014,7 @@
       <c r="AX279" s="1"/>
       <c r="AY279" s="1"/>
     </row>
-    <row r="280" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A280"/>
       <c r="B280" s="1"/>
       <c r="C280" s="1"/>
@@ -15067,7 +15064,7 @@
       <c r="AX280" s="1"/>
       <c r="AY280" s="1"/>
     </row>
-    <row r="281" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A281"/>
       <c r="B281" s="1"/>
       <c r="C281" s="1"/>
@@ -15117,7 +15114,7 @@
       <c r="AX281" s="1"/>
       <c r="AY281" s="1"/>
     </row>
-    <row r="282" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A282"/>
       <c r="B282" s="1"/>
       <c r="C282" s="1"/>
@@ -15167,7 +15164,7 @@
       <c r="AX282" s="1"/>
       <c r="AY282" s="1"/>
     </row>
-    <row r="283" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A283"/>
       <c r="B283" s="1"/>
       <c r="C283" s="1"/>
@@ -15217,7 +15214,7 @@
       <c r="AX283" s="1"/>
       <c r="AY283" s="1"/>
     </row>
-    <row r="284" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A284"/>
       <c r="B284" s="1"/>
       <c r="C284" s="1"/>
@@ -15267,7 +15264,7 @@
       <c r="AX284" s="1"/>
       <c r="AY284" s="1"/>
     </row>
-    <row r="285" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A285"/>
       <c r="B285" s="1"/>
       <c r="C285" s="1"/>
@@ -15317,7 +15314,7 @@
       <c r="AX285" s="1"/>
       <c r="AY285" s="1"/>
     </row>
-    <row r="286" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A286"/>
       <c r="B286" s="1"/>
       <c r="C286" s="1"/>
@@ -15367,7 +15364,7 @@
       <c r="AX286" s="1"/>
       <c r="AY286" s="1"/>
     </row>
-    <row r="287" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A287"/>
       <c r="B287" s="1"/>
       <c r="C287" s="1"/>
@@ -15417,7 +15414,7 @@
       <c r="AX287" s="1"/>
       <c r="AY287" s="1"/>
     </row>
-    <row r="288" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A288"/>
       <c r="B288" s="1"/>
       <c r="C288" s="1"/>
@@ -15467,7 +15464,7 @@
       <c r="AX288" s="1"/>
       <c r="AY288" s="1"/>
     </row>
-    <row r="289" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A289"/>
       <c r="B289" s="1"/>
       <c r="C289" s="1"/>
@@ -15517,7 +15514,7 @@
       <c r="AX289" s="1"/>
       <c r="AY289" s="1"/>
     </row>
-    <row r="290" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A290"/>
       <c r="B290" s="1"/>
       <c r="C290" s="1"/>
@@ -15567,7 +15564,7 @@
       <c r="AX290" s="1"/>
       <c r="AY290" s="1"/>
     </row>
-    <row r="291" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A291"/>
       <c r="B291" s="1"/>
       <c r="C291" s="1"/>
@@ -15617,7 +15614,7 @@
       <c r="AX291" s="1"/>
       <c r="AY291" s="1"/>
     </row>
-    <row r="292" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A292"/>
       <c r="B292" s="1"/>
       <c r="C292" s="1"/>
@@ -15667,7 +15664,7 @@
       <c r="AX292" s="1"/>
       <c r="AY292" s="1"/>
     </row>
-    <row r="293" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A293"/>
       <c r="B293" s="1"/>
       <c r="C293" s="1"/>
@@ -15717,7 +15714,7 @@
       <c r="AX293" s="1"/>
       <c r="AY293" s="1"/>
     </row>
-    <row r="294" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A294"/>
       <c r="B294" s="1"/>
       <c r="C294" s="1"/>
@@ -15767,7 +15764,7 @@
       <c r="AX294" s="1"/>
       <c r="AY294" s="1"/>
     </row>
-    <row r="295" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A295"/>
       <c r="B295" s="1"/>
       <c r="C295" s="1"/>
@@ -15817,7 +15814,7 @@
       <c r="AX295" s="1"/>
       <c r="AY295" s="1"/>
     </row>
-    <row r="296" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A296"/>
       <c r="B296" s="1"/>
       <c r="C296" s="1"/>
@@ -15867,7 +15864,7 @@
       <c r="AX296" s="1"/>
       <c r="AY296" s="1"/>
     </row>
-    <row r="297" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A297"/>
       <c r="B297" s="1"/>
       <c r="C297" s="1"/>
@@ -15917,7 +15914,7 @@
       <c r="AX297" s="1"/>
       <c r="AY297" s="1"/>
     </row>
-    <row r="298" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A298"/>
       <c r="B298" s="1"/>
       <c r="C298" s="1"/>
@@ -15967,7 +15964,7 @@
       <c r="AX298" s="1"/>
       <c r="AY298" s="1"/>
     </row>
-    <row r="299" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A299"/>
       <c r="B299" s="1"/>
       <c r="C299" s="1"/>
@@ -16017,7 +16014,7 @@
       <c r="AX299" s="1"/>
       <c r="AY299" s="1"/>
     </row>
-    <row r="300" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A300"/>
       <c r="B300" s="1"/>
       <c r="C300" s="1"/>
@@ -16067,7 +16064,7 @@
       <c r="AX300" s="1"/>
       <c r="AY300" s="1"/>
     </row>
-    <row r="301" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A301"/>
       <c r="B301" s="1"/>
       <c r="C301" s="1"/>
@@ -16117,7 +16114,7 @@
       <c r="AX301" s="1"/>
       <c r="AY301" s="1"/>
     </row>
-    <row r="302" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A302"/>
       <c r="B302" s="1"/>
       <c r="C302" s="1"/>
@@ -16167,7 +16164,7 @@
       <c r="AX302" s="1"/>
       <c r="AY302" s="1"/>
     </row>
-    <row r="303" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A303"/>
       <c r="B303" s="1"/>
       <c r="C303" s="1"/>
@@ -16217,7 +16214,7 @@
       <c r="AX303" s="1"/>
       <c r="AY303" s="1"/>
     </row>
-    <row r="304" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A304"/>
       <c r="B304" s="1"/>
       <c r="C304" s="1"/>
@@ -16267,7 +16264,7 @@
       <c r="AX304" s="1"/>
       <c r="AY304" s="1"/>
     </row>
-    <row r="305" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A305"/>
       <c r="B305" s="1"/>
       <c r="C305" s="1"/>
@@ -16317,7 +16314,7 @@
       <c r="AX305" s="1"/>
       <c r="AY305" s="1"/>
     </row>
-    <row r="306" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A306"/>
       <c r="B306" s="1"/>
       <c r="C306" s="1"/>
@@ -16367,7 +16364,7 @@
       <c r="AX306" s="1"/>
       <c r="AY306" s="1"/>
     </row>
-    <row r="307" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A307"/>
       <c r="B307" s="1"/>
       <c r="C307" s="1"/>
@@ -16417,7 +16414,7 @@
       <c r="AX307" s="1"/>
       <c r="AY307" s="1"/>
     </row>
-    <row r="308" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A308"/>
       <c r="B308" s="1"/>
       <c r="C308" s="1"/>
@@ -16467,7 +16464,7 @@
       <c r="AX308" s="1"/>
       <c r="AY308" s="1"/>
     </row>
-    <row r="309" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A309"/>
       <c r="B309" s="1"/>
       <c r="C309" s="1"/>
@@ -16517,7 +16514,7 @@
       <c r="AX309" s="1"/>
       <c r="AY309" s="1"/>
     </row>
-    <row r="310" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A310"/>
       <c r="B310" s="1"/>
       <c r="C310" s="1"/>
@@ -16567,7 +16564,7 @@
       <c r="AX310" s="1"/>
       <c r="AY310" s="1"/>
     </row>
-    <row r="311" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A311"/>
       <c r="B311" s="1"/>
       <c r="C311" s="1"/>
@@ -16617,7 +16614,7 @@
       <c r="AX311" s="1"/>
       <c r="AY311" s="1"/>
     </row>
-    <row r="312" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A312"/>
       <c r="B312" s="1"/>
       <c r="C312" s="1"/>
@@ -16667,7 +16664,7 @@
       <c r="AX312" s="1"/>
       <c r="AY312" s="1"/>
     </row>
-    <row r="313" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A313"/>
       <c r="B313" s="1"/>
       <c r="C313" s="1"/>
@@ -16717,7 +16714,7 @@
       <c r="AX313" s="1"/>
       <c r="AY313" s="1"/>
     </row>
-    <row r="314" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A314"/>
       <c r="B314" s="1"/>
       <c r="C314" s="1"/>
@@ -16767,7 +16764,7 @@
       <c r="AX314" s="1"/>
       <c r="AY314" s="1"/>
     </row>
-    <row r="315" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A315"/>
       <c r="B315" s="1"/>
       <c r="C315" s="1"/>
@@ -16817,7 +16814,7 @@
       <c r="AX315" s="1"/>
       <c r="AY315" s="1"/>
     </row>
-    <row r="316" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A316"/>
       <c r="B316" s="1"/>
       <c r="C316" s="1"/>
@@ -16867,7 +16864,7 @@
       <c r="AX316" s="1"/>
       <c r="AY316" s="1"/>
     </row>
-    <row r="317" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A317"/>
       <c r="B317" s="1"/>
       <c r="C317" s="1"/>
@@ -16917,7 +16914,7 @@
       <c r="AX317" s="1"/>
       <c r="AY317" s="1"/>
     </row>
-    <row r="318" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A318"/>
       <c r="B318" s="1"/>
       <c r="C318" s="1"/>
@@ -16967,7 +16964,7 @@
       <c r="AX318" s="1"/>
       <c r="AY318" s="1"/>
     </row>
-    <row r="319" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A319"/>
       <c r="B319" s="1"/>
       <c r="C319" s="1"/>
@@ -17017,7 +17014,7 @@
       <c r="AX319" s="1"/>
       <c r="AY319" s="1"/>
     </row>
-    <row r="320" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A320"/>
       <c r="B320" s="1"/>
       <c r="C320" s="1"/>
@@ -17067,7 +17064,7 @@
       <c r="AX320" s="1"/>
       <c r="AY320" s="1"/>
     </row>
-    <row r="321" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A321"/>
       <c r="B321" s="1"/>
       <c r="C321" s="1"/>
@@ -17117,7 +17114,7 @@
       <c r="AX321" s="1"/>
       <c r="AY321" s="1"/>
     </row>
-    <row r="322" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A322"/>
       <c r="B322" s="1"/>
       <c r="C322" s="1"/>
@@ -17167,7 +17164,7 @@
       <c r="AX322" s="1"/>
       <c r="AY322" s="1"/>
     </row>
-    <row r="323" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A323"/>
       <c r="B323" s="1"/>
       <c r="C323" s="1"/>
@@ -17217,7 +17214,7 @@
       <c r="AX323" s="1"/>
       <c r="AY323" s="1"/>
     </row>
-    <row r="324" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A324"/>
       <c r="B324" s="1"/>
       <c r="C324" s="1"/>
@@ -17267,7 +17264,7 @@
       <c r="AX324" s="1"/>
       <c r="AY324" s="1"/>
     </row>
-    <row r="325" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A325"/>
       <c r="B325" s="1"/>
       <c r="C325" s="1"/>
@@ -17317,7 +17314,7 @@
       <c r="AX325" s="1"/>
       <c r="AY325" s="1"/>
     </row>
-    <row r="326" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A326"/>
       <c r="B326" s="1"/>
       <c r="C326" s="1"/>
@@ -17367,7 +17364,7 @@
       <c r="AX326" s="1"/>
       <c r="AY326" s="1"/>
     </row>
-    <row r="327" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A327"/>
       <c r="B327" s="1"/>
       <c r="C327" s="1"/>
@@ -17417,7 +17414,7 @@
       <c r="AX327" s="1"/>
       <c r="AY327" s="1"/>
     </row>
-    <row r="328" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A328"/>
       <c r="B328" s="1"/>
       <c r="C328" s="1"/>
@@ -17467,7 +17464,7 @@
       <c r="AX328" s="1"/>
       <c r="AY328" s="1"/>
     </row>
-    <row r="329" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A329"/>
       <c r="B329" s="1"/>
       <c r="C329" s="1"/>
@@ -17517,7 +17514,7 @@
       <c r="AX329" s="1"/>
       <c r="AY329" s="1"/>
     </row>
-    <row r="330" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A330"/>
       <c r="B330" s="1"/>
       <c r="C330" s="1"/>
@@ -17567,7 +17564,7 @@
       <c r="AX330" s="1"/>
       <c r="AY330" s="1"/>
     </row>
-    <row r="331" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A331"/>
       <c r="B331" s="1"/>
       <c r="C331" s="1"/>
@@ -17617,7 +17614,7 @@
       <c r="AX331" s="1"/>
       <c r="AY331" s="1"/>
     </row>
-    <row r="332" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A332"/>
       <c r="B332" s="1"/>
       <c r="C332" s="1"/>
@@ -17667,7 +17664,7 @@
       <c r="AX332" s="1"/>
       <c r="AY332" s="1"/>
     </row>
-    <row r="333" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A333"/>
       <c r="B333" s="1"/>
       <c r="C333" s="1"/>
@@ -17717,7 +17714,7 @@
       <c r="AX333" s="1"/>
       <c r="AY333" s="1"/>
     </row>
-    <row r="334" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A334"/>
       <c r="B334" s="1"/>
       <c r="C334" s="1"/>
@@ -17767,7 +17764,7 @@
       <c r="AX334" s="1"/>
       <c r="AY334" s="1"/>
     </row>
-    <row r="335" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A335"/>
       <c r="B335" s="1"/>
       <c r="C335" s="1"/>
@@ -17817,7 +17814,7 @@
       <c r="AX335" s="1"/>
       <c r="AY335" s="1"/>
     </row>
-    <row r="336" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A336"/>
       <c r="B336" s="1"/>
       <c r="C336" s="1"/>
@@ -17867,7 +17864,7 @@
       <c r="AX336" s="1"/>
       <c r="AY336" s="1"/>
     </row>
-    <row r="337" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A337"/>
       <c r="B337" s="1"/>
       <c r="C337" s="1"/>
@@ -17917,7 +17914,7 @@
       <c r="AX337" s="1"/>
       <c r="AY337" s="1"/>
     </row>
-    <row r="338" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A338"/>
       <c r="B338" s="1"/>
       <c r="C338" s="1"/>
@@ -17967,7 +17964,7 @@
       <c r="AX338" s="1"/>
       <c r="AY338" s="1"/>
     </row>
-    <row r="339" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A339"/>
       <c r="B339" s="1"/>
       <c r="C339" s="1"/>
@@ -18017,7 +18014,7 @@
       <c r="AX339" s="1"/>
       <c r="AY339" s="1"/>
     </row>
-    <row r="340" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A340"/>
       <c r="B340" s="1"/>
       <c r="C340" s="1"/>
@@ -18067,7 +18064,7 @@
       <c r="AX340" s="1"/>
       <c r="AY340" s="1"/>
     </row>
-    <row r="341" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A341"/>
       <c r="B341" s="1"/>
       <c r="C341" s="1"/>
@@ -18117,7 +18114,7 @@
       <c r="AX341" s="1"/>
       <c r="AY341" s="1"/>
     </row>
-    <row r="342" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A342"/>
       <c r="B342" s="1"/>
       <c r="C342" s="1"/>
@@ -18167,7 +18164,7 @@
       <c r="AX342" s="1"/>
       <c r="AY342" s="1"/>
     </row>
-    <row r="343" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A343"/>
       <c r="B343" s="1"/>
       <c r="C343" s="1"/>
@@ -18217,7 +18214,7 @@
       <c r="AX343" s="1"/>
       <c r="AY343" s="1"/>
     </row>
-    <row r="344" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A344"/>
       <c r="B344" s="1"/>
       <c r="C344" s="1"/>
@@ -18267,7 +18264,7 @@
       <c r="AX344" s="1"/>
       <c r="AY344" s="1"/>
     </row>
-    <row r="345" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A345"/>
       <c r="B345" s="1"/>
       <c r="C345" s="1"/>
@@ -18317,7 +18314,7 @@
       <c r="AX345" s="1"/>
       <c r="AY345" s="1"/>
     </row>
-    <row r="346" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A346"/>
       <c r="B346" s="1"/>
       <c r="C346" s="1"/>
@@ -18367,7 +18364,7 @@
       <c r="AX346" s="1"/>
       <c r="AY346" s="1"/>
     </row>
-    <row r="347" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A347"/>
       <c r="B347" s="1"/>
       <c r="C347" s="1"/>
@@ -18417,7 +18414,7 @@
       <c r="AX347" s="1"/>
       <c r="AY347" s="1"/>
     </row>
-    <row r="348" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A348"/>
       <c r="B348" s="1"/>
       <c r="C348" s="1"/>
@@ -18467,7 +18464,7 @@
       <c r="AX348" s="1"/>
       <c r="AY348" s="1"/>
     </row>
-    <row r="349" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A349"/>
       <c r="B349" s="1"/>
       <c r="C349" s="1"/>
@@ -18517,7 +18514,7 @@
       <c r="AX349" s="1"/>
       <c r="AY349" s="1"/>
     </row>
-    <row r="350" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A350"/>
       <c r="B350" s="1"/>
       <c r="C350" s="1"/>
@@ -18567,7 +18564,7 @@
       <c r="AX350" s="1"/>
       <c r="AY350" s="1"/>
     </row>
-    <row r="351" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A351"/>
       <c r="B351" s="1"/>
       <c r="C351" s="1"/>
@@ -18617,7 +18614,7 @@
       <c r="AX351" s="1"/>
       <c r="AY351" s="1"/>
     </row>
-    <row r="352" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A352"/>
       <c r="B352" s="1"/>
       <c r="C352" s="1"/>
@@ -18667,7 +18664,7 @@
       <c r="AX352" s="1"/>
       <c r="AY352" s="1"/>
     </row>
-    <row r="353" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A353"/>
       <c r="B353" s="1"/>
       <c r="C353" s="1"/>
@@ -18717,7 +18714,7 @@
       <c r="AX353" s="1"/>
       <c r="AY353" s="1"/>
     </row>
-    <row r="354" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A354"/>
       <c r="B354" s="1"/>
       <c r="C354" s="1"/>
@@ -18767,7 +18764,7 @@
       <c r="AX354" s="1"/>
       <c r="AY354" s="1"/>
     </row>
-    <row r="355" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A355"/>
       <c r="B355" s="1"/>
       <c r="C355" s="1"/>
@@ -18817,7 +18814,7 @@
       <c r="AX355" s="1"/>
       <c r="AY355" s="1"/>
     </row>
-    <row r="356" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A356"/>
       <c r="B356" s="1"/>
       <c r="C356" s="1"/>
@@ -18867,7 +18864,7 @@
       <c r="AX356" s="1"/>
       <c r="AY356" s="1"/>
     </row>
-    <row r="357" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A357"/>
       <c r="B357" s="1"/>
       <c r="C357" s="1"/>
@@ -18917,7 +18914,7 @@
       <c r="AX357" s="1"/>
       <c r="AY357" s="1"/>
     </row>
-    <row r="358" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A358"/>
       <c r="B358" s="1"/>
       <c r="C358" s="1"/>
@@ -18967,7 +18964,7 @@
       <c r="AX358" s="1"/>
       <c r="AY358" s="1"/>
     </row>
-    <row r="359" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A359"/>
       <c r="B359" s="1"/>
       <c r="C359" s="1"/>
@@ -19017,7 +19014,7 @@
       <c r="AX359" s="1"/>
       <c r="AY359" s="1"/>
     </row>
-    <row r="360" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A360"/>
       <c r="B360" s="1"/>
       <c r="C360" s="1"/>
@@ -19067,7 +19064,7 @@
       <c r="AX360" s="1"/>
       <c r="AY360" s="1"/>
     </row>
-    <row r="361" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A361"/>
       <c r="B361" s="1"/>
       <c r="C361" s="1"/>
@@ -19117,7 +19114,7 @@
       <c r="AX361" s="1"/>
       <c r="AY361" s="1"/>
     </row>
-    <row r="362" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A362"/>
       <c r="B362" s="1"/>
       <c r="C362" s="1"/>
@@ -19167,7 +19164,7 @@
       <c r="AX362" s="1"/>
       <c r="AY362" s="1"/>
     </row>
-    <row r="363" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A363"/>
       <c r="B363" s="1"/>
       <c r="C363" s="1"/>
@@ -19217,7 +19214,7 @@
       <c r="AX363" s="1"/>
       <c r="AY363" s="1"/>
     </row>
-    <row r="364" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A364"/>
       <c r="B364" s="1"/>
       <c r="C364" s="1"/>
@@ -19267,7 +19264,7 @@
       <c r="AX364" s="1"/>
       <c r="AY364" s="1"/>
     </row>
-    <row r="365" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A365"/>
       <c r="B365" s="1"/>
       <c r="C365" s="1"/>
@@ -19317,7 +19314,7 @@
       <c r="AX365" s="1"/>
       <c r="AY365" s="1"/>
     </row>
-    <row r="366" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A366"/>
       <c r="B366" s="1"/>
       <c r="C366" s="1"/>
@@ -19367,7 +19364,7 @@
       <c r="AX366" s="1"/>
       <c r="AY366" s="1"/>
     </row>
-    <row r="367" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A367"/>
       <c r="B367" s="1"/>
       <c r="C367" s="1"/>
@@ -19417,7 +19414,7 @@
       <c r="AX367" s="1"/>
       <c r="AY367" s="1"/>
     </row>
-    <row r="368" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A368"/>
       <c r="B368" s="1"/>
       <c r="C368" s="1"/>
@@ -19467,7 +19464,7 @@
       <c r="AX368" s="1"/>
       <c r="AY368" s="1"/>
     </row>
-    <row r="369" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A369"/>
       <c r="B369" s="1"/>
       <c r="C369" s="1"/>
@@ -19517,7 +19514,7 @@
       <c r="AX369" s="1"/>
       <c r="AY369" s="1"/>
     </row>
-    <row r="370" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A370"/>
       <c r="B370" s="1"/>
       <c r="C370" s="1"/>
@@ -19567,7 +19564,7 @@
       <c r="AX370" s="1"/>
       <c r="AY370" s="1"/>
     </row>
-    <row r="371" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A371"/>
       <c r="B371" s="1"/>
       <c r="C371" s="1"/>
@@ -19617,7 +19614,7 @@
       <c r="AX371" s="1"/>
       <c r="AY371" s="1"/>
     </row>
-    <row r="372" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A372"/>
       <c r="B372" s="1"/>
       <c r="C372" s="1"/>
@@ -19667,7 +19664,7 @@
       <c r="AX372" s="1"/>
       <c r="AY372" s="1"/>
     </row>
-    <row r="373" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A373"/>
       <c r="B373" s="1"/>
       <c r="C373" s="1"/>
@@ -19717,7 +19714,7 @@
       <c r="AX373" s="1"/>
       <c r="AY373" s="1"/>
     </row>
-    <row r="374" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A374"/>
       <c r="B374" s="1"/>
       <c r="C374" s="1"/>
@@ -19767,7 +19764,7 @@
       <c r="AX374" s="1"/>
       <c r="AY374" s="1"/>
     </row>
-    <row r="375" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A375"/>
       <c r="B375" s="1"/>
       <c r="C375" s="1"/>
@@ -19817,7 +19814,7 @@
       <c r="AX375" s="1"/>
       <c r="AY375" s="1"/>
     </row>
-    <row r="376" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A376"/>
       <c r="B376" s="1"/>
       <c r="C376" s="1"/>
@@ -19867,7 +19864,7 @@
       <c r="AX376" s="1"/>
       <c r="AY376" s="1"/>
     </row>
-    <row r="377" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A377"/>
       <c r="B377" s="1"/>
       <c r="C377" s="1"/>
@@ -19917,7 +19914,7 @@
       <c r="AX377" s="1"/>
       <c r="AY377" s="1"/>
     </row>
-    <row r="378" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A378"/>
       <c r="B378" s="1"/>
       <c r="C378" s="1"/>
@@ -19967,7 +19964,7 @@
       <c r="AX378" s="1"/>
       <c r="AY378" s="1"/>
     </row>
-    <row r="379" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A379"/>
       <c r="B379" s="1"/>
       <c r="C379" s="1"/>
@@ -20017,7 +20014,7 @@
       <c r="AX379" s="1"/>
       <c r="AY379" s="1"/>
     </row>
-    <row r="380" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A380"/>
       <c r="B380" s="1"/>
       <c r="C380" s="1"/>
@@ -20067,7 +20064,7 @@
       <c r="AX380" s="1"/>
       <c r="AY380" s="1"/>
     </row>
-    <row r="381" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A381"/>
       <c r="B381" s="1"/>
       <c r="C381" s="1"/>
@@ -20117,7 +20114,7 @@
       <c r="AX381" s="1"/>
       <c r="AY381" s="1"/>
     </row>
-    <row r="382" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A382"/>
       <c r="B382" s="1"/>
       <c r="C382" s="1"/>
@@ -20167,7 +20164,7 @@
       <c r="AX382" s="1"/>
       <c r="AY382" s="1"/>
     </row>
-    <row r="383" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A383"/>
       <c r="B383" s="1"/>
       <c r="C383" s="1"/>
@@ -20217,7 +20214,7 @@
       <c r="AX383" s="1"/>
       <c r="AY383" s="1"/>
     </row>
-    <row r="384" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A384"/>
       <c r="B384" s="1"/>
       <c r="C384" s="1"/>
@@ -20267,7 +20264,7 @@
       <c r="AX384" s="1"/>
       <c r="AY384" s="1"/>
     </row>
-    <row r="385" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A385"/>
       <c r="B385" s="1"/>
       <c r="C385" s="1"/>
@@ -20317,7 +20314,7 @@
       <c r="AX385" s="1"/>
       <c r="AY385" s="1"/>
     </row>
-    <row r="386" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A386"/>
       <c r="B386" s="1"/>
       <c r="C386" s="1"/>
@@ -20367,7 +20364,7 @@
       <c r="AX386" s="1"/>
       <c r="AY386" s="1"/>
     </row>
-    <row r="387" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A387"/>
       <c r="B387" s="1"/>
       <c r="C387" s="1"/>
@@ -20417,7 +20414,7 @@
       <c r="AX387" s="1"/>
       <c r="AY387" s="1"/>
     </row>
-    <row r="388" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A388"/>
       <c r="B388" s="1"/>
       <c r="C388" s="1"/>
@@ -20467,7 +20464,7 @@
       <c r="AX388" s="1"/>
       <c r="AY388" s="1"/>
     </row>
-    <row r="389" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A389"/>
       <c r="B389" s="1"/>
       <c r="C389" s="1"/>
@@ -20517,7 +20514,7 @@
       <c r="AX389" s="1"/>
       <c r="AY389" s="1"/>
     </row>
-    <row r="390" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A390"/>
       <c r="B390" s="1"/>
       <c r="C390" s="1"/>
@@ -20567,7 +20564,7 @@
       <c r="AX390" s="1"/>
       <c r="AY390" s="1"/>
     </row>
-    <row r="391" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A391"/>
       <c r="B391" s="1"/>
       <c r="C391" s="1"/>
@@ -20617,7 +20614,7 @@
       <c r="AX391" s="1"/>
       <c r="AY391" s="1"/>
     </row>
-    <row r="392" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A392"/>
       <c r="B392" s="1"/>
       <c r="C392" s="1"/>
@@ -20667,7 +20664,7 @@
       <c r="AX392" s="1"/>
       <c r="AY392" s="1"/>
     </row>
-    <row r="393" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="393" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A393"/>
       <c r="B393" s="1"/>
       <c r="C393" s="1"/>
@@ -20717,7 +20714,7 @@
       <c r="AX393" s="1"/>
       <c r="AY393" s="1"/>
     </row>
-    <row r="394" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A394"/>
       <c r="B394" s="1"/>
       <c r="C394" s="1"/>
@@ -20767,7 +20764,7 @@
       <c r="AX394" s="1"/>
       <c r="AY394" s="1"/>
     </row>
-    <row r="395" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A395"/>
       <c r="B395" s="1"/>
       <c r="C395" s="1"/>
@@ -20817,7 +20814,7 @@
       <c r="AX395" s="1"/>
       <c r="AY395" s="1"/>
     </row>
-    <row r="396" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A396"/>
       <c r="B396" s="1"/>
       <c r="C396" s="1"/>
@@ -20867,7 +20864,7 @@
       <c r="AX396" s="1"/>
       <c r="AY396" s="1"/>
     </row>
-    <row r="397" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A397"/>
       <c r="B397" s="1"/>
       <c r="C397" s="1"/>
@@ -20917,7 +20914,7 @@
       <c r="AX397" s="1"/>
       <c r="AY397" s="1"/>
     </row>
-    <row r="398" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="398" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A398"/>
       <c r="B398" s="1"/>
       <c r="C398" s="1"/>
@@ -20967,7 +20964,7 @@
       <c r="AX398" s="1"/>
       <c r="AY398" s="1"/>
     </row>
-    <row r="399" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A399"/>
       <c r="B399" s="1"/>
       <c r="C399" s="1"/>
@@ -21017,7 +21014,7 @@
       <c r="AX399" s="1"/>
       <c r="AY399" s="1"/>
     </row>
-    <row r="400" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A400"/>
       <c r="B400" s="1"/>
       <c r="C400" s="1"/>
@@ -21067,7 +21064,7 @@
       <c r="AX400" s="1"/>
       <c r="AY400" s="1"/>
     </row>
-    <row r="401" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A401"/>
       <c r="B401" s="1"/>
       <c r="C401" s="1"/>
@@ -21117,7 +21114,7 @@
       <c r="AX401" s="1"/>
       <c r="AY401" s="1"/>
     </row>
-    <row r="402" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A402"/>
       <c r="B402" s="1"/>
       <c r="C402" s="1"/>
@@ -21167,7 +21164,7 @@
       <c r="AX402" s="1"/>
       <c r="AY402" s="1"/>
     </row>
-    <row r="403" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A403"/>
       <c r="B403" s="1"/>
       <c r="C403" s="1"/>
@@ -21217,7 +21214,7 @@
       <c r="AX403" s="1"/>
       <c r="AY403" s="1"/>
     </row>
-    <row r="404" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A404"/>
       <c r="B404" s="1"/>
       <c r="C404" s="1"/>
@@ -21267,7 +21264,7 @@
       <c r="AX404" s="1"/>
       <c r="AY404" s="1"/>
     </row>
-    <row r="405" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A405"/>
       <c r="B405" s="1"/>
       <c r="C405" s="1"/>
@@ -21317,7 +21314,7 @@
       <c r="AX405" s="1"/>
       <c r="AY405" s="1"/>
     </row>
-    <row r="406" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="406" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A406"/>
       <c r="B406" s="1"/>
       <c r="C406" s="1"/>
@@ -21367,7 +21364,7 @@
       <c r="AX406" s="1"/>
       <c r="AY406" s="1"/>
     </row>
-    <row r="407" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="407" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A407"/>
       <c r="B407" s="1"/>
       <c r="C407" s="1"/>
@@ -21417,7 +21414,7 @@
       <c r="AX407" s="1"/>
       <c r="AY407" s="1"/>
     </row>
-    <row r="408" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="408" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A408"/>
       <c r="B408" s="1"/>
       <c r="C408" s="1"/>
@@ -21467,7 +21464,7 @@
       <c r="AX408" s="1"/>
       <c r="AY408" s="1"/>
     </row>
-    <row r="409" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="409" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A409"/>
       <c r="B409" s="1"/>
       <c r="C409" s="1"/>
@@ -21517,7 +21514,7 @@
       <c r="AX409" s="1"/>
       <c r="AY409" s="1"/>
     </row>
-    <row r="410" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="410" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A410"/>
       <c r="B410" s="1"/>
       <c r="C410" s="1"/>
@@ -21567,7 +21564,7 @@
       <c r="AX410" s="1"/>
       <c r="AY410" s="1"/>
     </row>
-    <row r="411" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="411" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A411"/>
       <c r="B411" s="1"/>
       <c r="C411" s="1"/>
@@ -21617,7 +21614,7 @@
       <c r="AX411" s="1"/>
       <c r="AY411" s="1"/>
     </row>
-    <row r="412" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="412" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A412"/>
       <c r="B412" s="1"/>
       <c r="C412" s="1"/>
@@ -21667,7 +21664,7 @@
       <c r="AX412" s="1"/>
       <c r="AY412" s="1"/>
     </row>
-    <row r="413" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="413" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A413"/>
       <c r="B413" s="1"/>
       <c r="C413" s="1"/>
@@ -21717,7 +21714,7 @@
       <c r="AX413" s="1"/>
       <c r="AY413" s="1"/>
     </row>
-    <row r="414" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="414" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A414"/>
       <c r="B414" s="1"/>
       <c r="C414" s="1"/>
@@ -21767,7 +21764,7 @@
       <c r="AX414" s="1"/>
       <c r="AY414" s="1"/>
     </row>
-    <row r="415" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="415" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A415"/>
       <c r="B415" s="1"/>
       <c r="C415" s="1"/>
@@ -21817,7 +21814,7 @@
       <c r="AX415" s="1"/>
       <c r="AY415" s="1"/>
     </row>
-    <row r="416" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="416" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A416"/>
       <c r="B416" s="1"/>
       <c r="C416" s="1"/>
@@ -21867,7 +21864,7 @@
       <c r="AX416" s="1"/>
       <c r="AY416" s="1"/>
     </row>
-    <row r="417" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="417" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A417"/>
       <c r="B417" s="1"/>
       <c r="C417" s="1"/>
@@ -21949,17 +21946,23 @@
     <hyperlink ref="G14" r:id="rId2" location="70cdb3,https://github.com/Mudasir-Ahmad011/Route-Optimization-System" xr:uid="{A3892D4A-49F3-4B4B-B4CA-AFC5588916F9}"/>
     <hyperlink ref="G17" r:id="rId3" xr:uid="{22E55DF4-82B5-4E47-B367-2531DBE4B2D9}"/>
     <hyperlink ref="G10" r:id="rId4" xr:uid="{3F53EEDE-49FC-477F-89D5-C27FEA47F483}"/>
+    <hyperlink ref="G7" r:id="rId5" xr:uid="{23530D64-107E-43F9-87E3-F02673D0DEE5}"/>
+    <hyperlink ref="G16" r:id="rId6" xr:uid="{76F70C27-4BFF-4AE8-9A6A-0FCC25A7DC6A}"/>
+    <hyperlink ref="G13" r:id="rId7" xr:uid="{4E9B5472-21CC-41DC-9172-E5BF7243760B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
-  <drawing r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
+  <drawing r:id="rId9"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22180,27 +22183,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC69FD84-4722-485B-95F5-B25971BB4485}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8166D80B-5C7E-4401-9B25-09A4D3E293DD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="675b2d5a-2a5b-4198-b316-84224b1699b9"/>
-    <ds:schemaRef ds:uri="9926c504-9366-4d27-ba67-e7df4b72c3ca"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -22225,9 +22216,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8166D80B-5C7E-4401-9B25-09A4D3E293DD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC69FD84-4722-485B-95F5-B25971BB4485}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="675b2d5a-2a5b-4198-b316-84224b1699b9"/>
+    <ds:schemaRef ds:uri="9926c504-9366-4d27-ba67-e7df4b72c3ca"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>